<commit_message>
Ajustado o termo 'Condictions'
Ajustado o termo 'Condictions' para 'Conditions'
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Antec Recebíveis.xlsx
+++ b/DicionarioDeDados-Antec Recebíveis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A7E18A-23AB-494F-9872-1AB55240F06A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9AEF62-CF59-4463-927A-6482026BBC54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AntecRecebíveisPF" sheetId="10" r:id="rId1"/>
@@ -179,9 +179,6 @@
 14. não aplicável</t>
   </si>
   <si>
-    <t>termsCondictions</t>
-  </si>
-  <si>
     <t>Percentual que incide sobre a composição da  taxa de juros remuneratórias</t>
   </si>
   <si>
@@ -841,6 +838,9 @@
   </si>
   <si>
     <t>^(\d{1,9}\,\d{2}){1}$</t>
+  </si>
+  <si>
+    <t>termsConditions</t>
   </si>
 </sst>
 </file>
@@ -1364,11 +1364,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1467,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -1501,7 +1501,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -1513,10 +1513,10 @@
         <v>14</v>
       </c>
       <c r="G4" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>203</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>204</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -1537,7 +1537,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>19</v>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -1570,7 +1570,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
@@ -1589,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -1602,7 +1602,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -1621,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1630,10 +1630,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/chargingTriggerInfo</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -1652,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1662,10 +1662,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/type</v>
       </c>
       <c r="B9" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>220</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>221</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>19</v>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -1687,7 +1687,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -1697,10 +1697,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/value</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" s="34" t="s">
         <v>224</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>225</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>13</v>
@@ -1712,7 +1712,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="5">
@@ -1722,7 +1722,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -1747,10 +1747,10 @@
         <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>209</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>210</v>
       </c>
       <c r="I11" s="5">
         <v>0</v>
@@ -1759,7 +1759,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -1769,10 +1769,10 @@
         <v>openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/priceInfo</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>226</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>227</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -1791,10 +1791,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -1804,10 +1804,10 @@
         <v>openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
       </c>
       <c r="B13" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>229</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>230</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>13</v>
@@ -1826,23 +1826,23 @@
         <v>1</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B14)</f>
+        <f t="shared" ref="A14:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B14)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/rate</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -1854,20 +1854,20 @@
         <v>14</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="13">
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B15)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/referencialRate</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1886,20 +1886,20 @@
         <v>14</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B16)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/indexer</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1923,13 +1923,13 @@
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B17)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/prePostTax</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1948,29 +1948,29 @@
         <v>14</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H17" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>213</v>
-      </c>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B18)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/frequency</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>19</v>
@@ -1982,29 +1982,29 @@
         <v>14</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="25" t="s">
-        <v>215</v>
-      </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B19)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -2033,10 +2033,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>19</v>
@@ -2062,13 +2062,13 @@
     <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B21)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/termsCondictions</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/termsConditions</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
@@ -2162,11 +2162,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2265,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
@@ -2299,7 +2299,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -2311,10 +2311,10 @@
         <v>14</v>
       </c>
       <c r="G4" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>203</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>204</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -2335,7 +2335,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>19</v>
@@ -2348,13 +2348,13 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>217</v>
-      </c>
-      <c r="I5" s="13">
-        <v>1</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>218</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="28"/>
@@ -2368,7 +2368,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -2400,7 +2400,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -2419,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2428,10 +2428,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/chargingTriggerInfo</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -2450,7 +2450,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -2460,10 +2460,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/type</v>
       </c>
       <c r="B9" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>220</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>221</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>19</v>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -2485,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -2495,10 +2495,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/value</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" s="34" t="s">
         <v>224</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>225</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>13</v>
@@ -2510,7 +2510,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="5">
@@ -2520,7 +2520,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -2545,10 +2545,10 @@
         <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>209</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>210</v>
       </c>
       <c r="I11" s="5">
         <v>0</v>
@@ -2557,7 +2557,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -2567,10 +2567,10 @@
         <v>openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/priceInfo</v>
       </c>
       <c r="B12" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>226</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>227</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -2589,10 +2589,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -2602,10 +2602,10 @@
         <v>openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
       </c>
       <c r="B13" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>229</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>230</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>13</v>
@@ -2624,23 +2624,23 @@
         <v>1</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B14)</f>
+        <f t="shared" ref="A14:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B14)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/rate</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
@@ -2652,18 +2652,18 @@
         <v>14</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B15)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/referencialRate</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2682,20 +2682,20 @@
         <v>14</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B16)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/indexer</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2719,13 +2719,13 @@
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B17)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/prePostTax</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2744,27 +2744,27 @@
         <v>14</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B18)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/frequency</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>19</v>
@@ -2781,20 +2781,20 @@
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B19)</f>
+        <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -2823,10 +2823,10 @@
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>19</v>
@@ -2854,13 +2854,13 @@
     <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B21)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/termsCondictions</v>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/termsConditions</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>13</v>
@@ -2965,112 +2965,112 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3094,163 +3094,163 @@
   <sheetData>
     <row r="1" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -3260,142 +3260,142 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -3433,157 +3433,157 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
@@ -3593,172 +3593,172 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
@@ -3768,12 +3768,12 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusão/Ajuste de domínios e descrições
Revisados os nomes, Xpath, domínios (retirada de numeração), qtdes mínimas e máximas e ajustes estéticos do dicionário.
Inclusão e ajuste de domínios em base ao definido junto aos DOs e documentos do Bacen 3040 e 4015.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Antec Recebíveis.xlsx
+++ b/DicionarioDeDados-Antec Recebíveis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9AEF62-CF59-4463-927A-6482026BBC54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89B3FB34-2F80-4EA5-A817-36677073D240}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AntecRecebíveisPF" sheetId="10" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="231">
   <si>
     <t>Xpath</t>
   </si>
@@ -158,25 +158,6 @@
   </si>
   <si>
     <t>incomeRateInfo</t>
-  </si>
-  <si>
-    <t>opcional</t>
-  </si>
-  <si>
-    <t>1. cessão de direitos creditórios
-2. caução
-3. penhor
-4. alienação fiduciária
-5. hipoteca
-6. operações garantidas pelo governo
-7. outras garantias não fidejussórias
-8. seguros e assemelhados
-9. garantia fidejussória
-10. bens arrendados
-11. garantias internacionais
-12. operações garantidas por outras entidades
-13. acordos de compensação
-14. não aplicável</t>
   </si>
   <si>
     <t>Percentual que incide sobre a composição da  taxa de juros remuneratórias</t>
@@ -731,8 +712,80 @@
     <t>Números de 0 a 9 sem formatação</t>
   </si>
   <si>
+    <t>Sigla de identificação do serviço relacionado à Modalidade de direitos creditórios descontados, para pessoa física. Campo aberto. P. ex.  (Trazer a Exemplo)</t>
+  </si>
+  <si>
+    <t>Fatores geradores de cobrança que incidem sobre as Modalidades de direitos creditórios descontados, para pessoa física. Campo Livre Trazer Exemplo</t>
+  </si>
+  <si>
+    <t>^(\W{3}){1}$</t>
+  </si>
+  <si>
+    <t>moeda (ISO-4217)</t>
+  </si>
+  <si>
+    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1}</t>
+  </si>
+  <si>
+    <t>^(\d{1})$</t>
+  </si>
+  <si>
+    <t>^(a\.[d,m,a]\.){1}$</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>chargingTriggerInfo</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indica os tipos: mínimo, médio e máximo do valor informado. P.ex.'mínimo' </t>
+  </si>
+  <si>
+    <t>Mínimo
+Médio
+Máximo</t>
+  </si>
+  <si>
+    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para o item priceInfo</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Valor da tarifa cobrada, relativa ao serviço ofertado para a Modalidade de Empréstimo, para pessoa jurídica. P.ex. 45,00</t>
+  </si>
+  <si>
+    <t>Descrição de como é composto o valor da tarifa. p.ex. '0,25% sobre o excedente do limite acima de R$ 500,00'</t>
+  </si>
+  <si>
+    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para os itens: value, currency e type</t>
+  </si>
+  <si>
+    <t>changingUnit</t>
+  </si>
+  <si>
+    <t>Unidade ou forma de cobrança. P.ex. 'Por mês'</t>
+  </si>
+  <si>
+    <t>este campo sempre deverá estar preenchido</t>
+  </si>
+  <si>
+    <t>^(\d{1,9}\,\d{2}){1}$</t>
+  </si>
+  <si>
+    <t>termsConditions</t>
+  </si>
+  <si>
+    <t>additionalInfo</t>
+  </si>
+  <si>
     <r>
-      <t>Modalidades de direitos creditórios descontados ofertados para pessoas Físicas, conforme Circular 4015-Bacen. Direito creditório descontado é a antecipação de créditos relativos por ex. ao: desconto de duplicatas, desconto de cheques,antecipação de fatura de cartão de crédito</t>
+      <t xml:space="preserve">Modalidades de direitos creditórios descontados ofertados para pessoas jurídicas, conforme Circular 4015-Bacen. Direito creditório descontado é a antecipação de créditos relativos por ex. ao: desconto de duplicatas, desconto de cheques,antecipação de fatura de cartão de crédito
+</t>
     </r>
     <r>
       <rPr>
@@ -742,122 +795,222 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t/>
+      <t>desconto de duplicatas:</t>
     </r>
-  </si>
-  <si>
-    <t>desconto de duplicatas 
-desconto de cheques
-antecipação de fatura de cartão de crédito,
-outros direitos creditórios descontados
-outros títulos descontados</t>
-  </si>
-  <si>
-    <t>Sigla de identificação do serviço relacionado à Modalidade de direitos creditórios descontados, para pessoa física. Campo aberto. P. ex.  (Trazer a Exemplo)</t>
-  </si>
-  <si>
-    <t>Fatores geradores de cobrança que incidem sobre as Modalidades de direitos creditórios descontados, para pessoa física. Campo Livre Trazer Exemplo</t>
-  </si>
-  <si>
-    <t>^(\W{3}){1}$</t>
-  </si>
-  <si>
-    <t>moeda (ISO-4217)</t>
-  </si>
-  <si>
-    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1}</t>
-  </si>
-  <si>
-    <t>^(\d{1})$</t>
-  </si>
-  <si>
-    <t>0. Pré
-1. Pós</t>
-  </si>
-  <si>
-    <t>^(a\.[d,m,a]\.){1}$</t>
-  </si>
-  <si>
-    <t>'a.d.'
-'a.m.'
-'a.a.'</t>
-  </si>
-  <si>
-    <t>Modalidades de direitos creditórios descontados ofertados para pessoas jurídicas, conforme Circular 4015-Bacen. Direito creditório descontado é a antecipação de créditos relativos por ex. ao: desconto de duplicatas, desconto de cheques,antecipação de fatura de cartão de crédito</t>
-  </si>
-  <si>
-    <t>desconto de duplicatas 
-desconto de cheques
-antecipação de fatura de cartão de crédito
-outros direitos creditórios descontados
-outros títulos descontados</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>chargingTriggerInfo</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indica os tipos: mínimo, médio e máximo do valor informado. P.ex.'mínimo' </t>
-  </si>
-  <si>
-    <t>Mínimo
-Médio
-Máximo</t>
-  </si>
-  <si>
-    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para o item priceInfo</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Valor da tarifa cobrada, relativa ao serviço ofertado para a Modalidade de Empréstimo, para pessoa jurídica. P.ex. 45,00</t>
-  </si>
-  <si>
-    <t>priceInfo</t>
-  </si>
-  <si>
-    <t>Descrição de como é composto o valor da tarifa. p.ex. '0,25% sobre o excedente do limite acima de R$ 500,00'</t>
-  </si>
-  <si>
-    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para os itens: value, currency e type</t>
-  </si>
-  <si>
-    <t>changingUnit</t>
-  </si>
-  <si>
-    <t>Unidade ou forma de cobrança. P.ex. 'Por mês'</t>
-  </si>
-  <si>
-    <t>este campo sempre deverá estar preenchido</t>
-  </si>
-  <si>
-    <t>^(\d{1,9}\,\d{2}){1}$</t>
-  </si>
-  <si>
-    <t>termsConditions</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a duplicatas mercantis</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+desconto de cheques: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a cheques custodiados</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+antecipação de recebíveis de cartão de crédito: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>operações de crédito para adiantamento de recursos às pessoas jurídicas com base em fluxo de caixa futuro vinculado a direitos creditórios sob a forma de faturas de cartão de crédito</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+desconto de nota promissória: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>operação</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de crédito que permite antecipar o valor da venda a prazo dos produtos ou serviços mediante desconto de nota promissória</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modalidades de direitos creditórios descontados ofertados para pessoas Físicas, conforme Circular 4015-Bacen. Direito creditório descontado é a antecipação de créditos relativos por ex. ao: desconto de duplicatas, desconto de cheques,antecipação de fatura de cartão de crédito
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desconto de duplicatas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a duplicatas mercantis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desconto de cheques:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a cheques custodiados
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">antecipação de recebíveis de cartão de crédito: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">operações de crédito para adiantamento de recursos às pessoas jurídicas com base em fluxo de caixa futuro vinculado a direitos creditórios sob a forma de faturas de cartão de crédito
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">desconto de nota promissória: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>operação  de crédito que permite antecipar o valor da venda a prazo dos produtos ou serviços mediante desconto de nota promissória</t>
+    </r>
+  </si>
+  <si>
+    <t>Cessão de direitos creditórios
+Caução
+Penhor
+Alienação fiduciária
+Hipoteca
+Operações garantidas pelo governo
+Outras garantias não fidejussórias
+Seguros e assemelhados
+Garantia fidejussória
+Bens arrendados
+Garantias internacionais
+Operações garantidas por outras entidades
+Acordos de compensação
+Não aplicável</t>
+  </si>
+  <si>
+    <t>a.d.
+a.m.
+a.a.</t>
+  </si>
+  <si>
+    <t>Pré
+Pós</t>
+  </si>
+  <si>
+    <t>Desconto de duplicatas 
+Desconto de cheques
+Antecipação de recebíveis de cartão de crédito
+Desconto de nota promissória</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -869,73 +1022,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10.5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -965,33 +1064,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1001,86 +1075,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1373,80 +1415,80 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="29" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="71" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.85546875" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="19"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="str">
+      <c r="A2" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/name</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="12">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="13">
         <v>1</v>
       </c>
@@ -1456,67 +1498,67 @@
       <c r="K2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="str">
+      <c r="A3" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/name</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="12">
         <v>30</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="13">
         <v>1</v>
       </c>
       <c r="J3" s="13">
         <v>1</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="str">
+      <c r="A4" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/cnpjNumber</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="12">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="29">
-        <v>14</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>203</v>
+      <c r="H4" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -1528,60 +1570,60 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="str">
+    <row r="5" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B5)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/types</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="15">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="6" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
       </c>
       <c r="J5" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="28"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="str">
+      <c r="A6" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B6)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/serviceName</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="12">
         <v>50</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="6"/>
@@ -1589,467 +1631,467 @@
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/",B7)</f>
-        <v>openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/serviceCode</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="5" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B7)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/serviceCode</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="12">
         <v>30</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="str">
+      <c r="A8" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B8)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/chargingTriggerInfo</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>218</v>
+      <c r="B8" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="12">
         <v>2000</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="str">
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/",B9)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/type</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="12">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="G9" s="5"/>
+      <c r="H9" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="I9" s="17">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="17">
         <v>3</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="str">
+        <v>214</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
         <f t="shared" ref="A10:A11" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/",B10)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/value</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="12">
         <v>12</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5">
+      <c r="G10" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="17">
         <v>0</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="17">
         <v>3</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="str">
+        <v>214</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/currency</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="12">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11" s="33" t="s">
+      <c r="G11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>3</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B12)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/additionalInfo</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="12">
+        <v>80</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>3</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/priceInfo</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="K12" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B13)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="29">
-        <v>80</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="E13" s="12">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;organisations&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="29">
-        <v>50</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="5">
+      <c r="H13" s="14"/>
+      <c r="I13" s="17">
         <v>1</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>217</v>
+      <c r="J13" s="17" t="s">
+        <v>209</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L13" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="str">
+      <c r="A14" s="4" t="str">
         <f t="shared" ref="A14:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B14)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/rate</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="12">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="H14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="13">
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="str">
+      <c r="A15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/referencialRate</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="12">
         <v>7</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="H15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="str">
+      <c r="A16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/indexer</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="12">
         <v>30</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="13">
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="str">
+      <c r="A17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/prePostTax</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="12">
         <v>1</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>212</v>
+      <c r="G17" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>229</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="str">
+      <c r="A18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/frequency</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="15" t="s">
+      <c r="C18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="12">
         <v>4</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>214</v>
+      <c r="G18" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>228</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="str">
+      <c r="A19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D19" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="12">
         <v>1000</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="13">
         <v>0</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="213.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="str">
+    <row r="20" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B20)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="B20" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="12">
         <v>50</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="22" t="s">
-        <v>35</v>
+      <c r="G20" s="5"/>
+      <c r="H20" s="14" t="s">
+        <v>227</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -2060,29 +2102,29 @@
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="str">
+      <c r="A21" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B21)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/termsConditions</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="B21" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="12">
         <v>2000</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="24"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="13">
         <v>0</v>
       </c>
@@ -2093,64 +2135,64 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="24"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="24"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="14"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="6"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="24"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="24"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="24"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="24"/>
+      <c r="D27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2162,7 +2204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2171,80 +2213,80 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="167.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="44" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="73.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="44" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.85546875" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="19"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="str">
+      <c r="A2" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/",B2)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/name</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="13">
         <v>1</v>
       </c>
@@ -2254,67 +2296,67 @@
       <c r="K2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="28"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="str">
+      <c r="A3" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B3)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/name</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>30</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="13">
         <v>1</v>
       </c>
       <c r="J3" s="13">
         <v>1</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="str">
+      <c r="A4" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B4)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/cnpjNumber</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>14</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>203</v>
+      <c r="G4" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -2326,60 +2368,60 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="str">
+    <row r="5" spans="1:12" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B5)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/types</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="15">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="6" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="28"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="str">
+      <c r="A6" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B6)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/serviceName</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>50</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="6"/>
@@ -2387,461 +2429,460 @@
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/",B7)</f>
-        <v>openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/serviceCode</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="5" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B7)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/serviceCode</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>30</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="str">
+      <c r="A8" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B8)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/chargingTriggerInfo</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>218</v>
+      <c r="B8" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>2000</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="13">
         <v>1</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="str">
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/",B9)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/type</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="12">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="G9" s="5"/>
+      <c r="H9" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="I9" s="13">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="13">
         <v>3</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="str">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
         <f t="shared" ref="A10:A11" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/",B10)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/value</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="12">
         <v>12</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5">
+      <c r="G10" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="13">
         <v>0</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="13">
         <v>3</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="str">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/currency</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="12">
         <v>3</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11" s="33" t="s">
+      <c r="G11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <v>3</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B12)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/additionalInfo</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="12">
+        <v>80</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>3</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/priceInfo</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>225</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="K12" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B13)</f>
+        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="29">
-        <v>80</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="E13" s="12">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;organisations&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="29">
-        <v>50</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="5">
+      <c r="H13" s="14"/>
+      <c r="I13" s="13">
         <v>1</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>217</v>
+      <c r="J13" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L13" s="2"/>
+        <v>221</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="str">
+      <c r="A14" s="4" t="str">
         <f t="shared" ref="A14:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B14)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/rate</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="str">
+      <c r="A15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/referencialRate</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>7</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="str">
+      <c r="A16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/indexer</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>30</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="13">
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="str">
+      <c r="A17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/prePostTax</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>1</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>229</v>
+      </c>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="str">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/frequency</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="15" t="s">
+      <c r="C18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>30</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="str">
+      <c r="A19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>1000</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="13">
         <v>0</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="str">
+    <row r="20" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B20)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="B20" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="12">
         <v>50</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="22" t="s">
-        <v>35</v>
+      <c r="H20" s="14" t="s">
+        <v>227</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -2852,29 +2893,29 @@
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="str">
+      <c r="A21" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B21)</f>
         <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/termsConditions</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="B21" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>2000</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="24"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="13">
         <v>0</v>
       </c>
@@ -2885,64 +2926,64 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="24"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="24"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="14"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="6"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="24"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="24"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="24"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="24"/>
+      <c r="D27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2965,112 +3006,112 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3088,692 +3129,692 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46" style="12" customWidth="1"/>
+    <col min="1" max="1" width="46" style="3" customWidth="1"/>
     <col min="2" max="2" width="85" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="10" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="e" cm="1">
+      <c r="A61" s="3" t="e" cm="1">
         <f t="array" ref="A61">- Crédito pessoal consignado para servidores públicos: Operações de Crédito pessoal consignado</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>122</v>
+      <c r="A62" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="e" cm="1">
+      <c r="A63" s="3" t="e" cm="1">
         <f t="array" ref="A63">- Crédito pessoal consignado para trabalhadores do setor privado: Operações de Crédito</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>123</v>
+      <c r="A64" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="12">
+      <c r="A65" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="e" cm="1">
+      <c r="A66" s="3" t="e" cm="1">
         <f t="array" ref="A66">- Crédito pessoal consignado para beneficiários do INSS: Operações de Crédito pessoal</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12" t="s">
+      <c r="A67" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="12" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="12" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="12" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="12" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="12" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="12" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="12" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="12" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="12" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="12" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="12" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="12" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="12" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="12" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="12" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="12" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="12" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="12" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="12" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="12" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="12" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="12" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes após consderações do GT de Dados
1.	Foi substituído o termo ‘organisation’ por ‘brand’
2.	Mantido Tipo ‘Texto’ para atributos ENUM
3.	Ajustado Dicionário de Canais Eletrônicos
4.	Montado Dicionário de Canais Telefônicos
5.	Dicionário de Contas:
a.	Foi incluído campo ‘addtionalInfo’ para complementar opção ‘Outros’ do atributo Canais disponíveis para abertura e encerramento de contas
6.	Dicionário de Cartões:
a.	foram incluídos campos de informações complementares sempre que o ENUM traz opção: Outros
b.	foi alterado o nome do campo ‘brandCode’ para ‘creditCardNetwork’
7.	Dicionário de Empréstimos – relação de modalidades de empréstimos foram ajustados os nomes trazendo o prefixo ‘Empréstimo’, quando necessário
8.	Dicionário de Financiamentos – relação de modalidades de financiamentos foram ajustados os nomes trazendo o prefixo ‘Financiamento’, ‘Financiamento rural-’ e ‘Financiamento imobiliário-‘ quando necessário.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Antec Recebíveis.xlsx
+++ b/DicionarioDeDados-Antec Recebíveis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89B3FB34-2F80-4EA5-A817-36677073D240}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AD477B-29DD-4882-9D3C-020BF6C19B37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AntecRecebíveisPF" sheetId="10" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="231">
   <si>
     <t>Xpath</t>
   </si>
@@ -94,9 +94,6 @@
     <t>name</t>
   </si>
   <si>
-    <t xml:space="preserve">Nome do conglomerado. P.ex. 'Organização A' </t>
-  </si>
-  <si>
     <t>Texto</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>types</t>
   </si>
   <si>
-    <t>Enum</t>
-  </si>
-  <si>
     <t>serviceName</t>
   </si>
   <si>
@@ -160,13 +154,7 @@
     <t>incomeRateInfo</t>
   </si>
   <si>
-    <t>Percentual que incide sobre a composição da  taxa de juros remuneratórias</t>
-  </si>
-  <si>
     <t>^(-?\d{1,2}){1}(\,\d{1,2}){1}$</t>
-  </si>
-  <si>
-    <t>^(-?\d{1,14}){1}(\,\d{1,4}){1}$</t>
   </si>
   <si>
     <t>Frequência sobre a qual incide a Remuneração. P. ex. 'a.d', 'a.m.', a.a.'</t>
@@ -626,13 +614,6 @@
   </si>
   <si>
     <t>requiredWarranties</t>
-  </si>
-  <si>
-    <t>Nome da Instituição, pertencente à organização, responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Jurídicas cosultadas. Ex. 'Empresa da Organização A'</t>
-  </si>
-  <si>
-    <t>O responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Jurídicas cosultadas - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. Composto por: os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Os quatro seguintes números de ordem das filiais da empresa. Normalmente a empresa matriz tem este campo preenchido com '0001'. Os dois últimos números correspondem ao dígito verificador.  composição do CNPJ pode ser assim representada, conforme ex. '50.685.362/0001-35' 
-Deve-se ter apenas os números do CNPJ, sem máscara.</t>
   </si>
   <si>
     <t>Nomes das Tarifas cobradas sobre Serviços ofertados à Modalidade de direitos creditórios descontados, para pessoa física. (Campo Livre) (trazer exemplo)</t>
@@ -696,91 +677,202 @@
     </r>
   </si>
   <si>
-    <t>Nome da Instituição, pertencente à organização, responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Físicas cosultadas. Ex. 'Empresa da Organização A'</t>
-  </si>
-  <si>
-    <t>O responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Físicas cosultadas - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa física. Composto por: os oito primeiros números à esquerda (XX. XXX. XXX) formam a "raiz" ou base, que identifica a empresa de forma única. Os quatro seguintes números de ordem das filiais da empresa. Normalmente a empresa matriz tem este campo preenchido com '0001'. Os dois últimos números correspondem ao dígito verificador.  composição do CNPJ pode ser assim representada, conforme ex. '50.685.362/0001-35' 
+    <t>Descrição da Remuneração relativa as taxas de juros remuneratórias sobre a modalidade de direitos creditórios descontados infomrada, para pessoa física</t>
+  </si>
+  <si>
+    <t>^(\d{14})$</t>
+  </si>
+  <si>
+    <t>Sigla de identificação do serviço relacionado à Modalidade de direitos creditórios descontados, para pessoa física. Campo aberto. P. ex.  (Trazer a Exemplo)</t>
+  </si>
+  <si>
+    <t>Fatores geradores de cobrança que incidem sobre as Modalidades de direitos creditórios descontados, para pessoa física. Campo Livre Trazer Exemplo</t>
+  </si>
+  <si>
+    <t>^(\W{3}){1}$</t>
+  </si>
+  <si>
+    <t>moeda (ISO-4217)</t>
+  </si>
+  <si>
+    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1}</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>chargingTriggerInfo</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Descrição de como é composto o valor da tarifa. p.ex. '0,25% sobre o excedente do limite acima de R$ 500,00'</t>
+  </si>
+  <si>
+    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para os itens: value, currency e type</t>
+  </si>
+  <si>
+    <t>changingUnit</t>
+  </si>
+  <si>
+    <t>Unidade ou forma de cobrança. P.ex. 'Por mês'</t>
+  </si>
+  <si>
+    <t>este campo sempre deverá estar preenchido</t>
+  </si>
+  <si>
+    <t>^(\d{1,9}\,\d{2}){1}$</t>
+  </si>
+  <si>
+    <t>termsConditions</t>
+  </si>
+  <si>
+    <t>additionalInfo</t>
+  </si>
+  <si>
+    <t>Cessão de direitos creditórios
+Caução
+Penhor
+Alienação fiduciária
+Hipoteca
+Operações garantidas pelo governo
+Outras garantias não fidejussórias
+Seguros e assemelhados
+Garantia fidejussória
+Bens arrendados
+Garantias internacionais
+Operações garantidas por outras entidades
+Acordos de compensação
+Não aplicável</t>
+  </si>
+  <si>
+    <t>a.d.
+a.m.
+a.a.</t>
+  </si>
+  <si>
+    <t>Pré
+Pós</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modalidades de direitos creditórios descontados ofertados para pessoas Físicas, conforme Circular 4015-Bacen. Direito creditório descontado é a antecipação de créditos relativos por ex. ao: desconto de duplicatas, desconto de cheques,antecipação de fatura de cartão de crédito
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desconto de duplicatas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a duplicatas mercantis
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>desconto de cheques:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a cheques custodiados
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">antecipação de fatura de cartão de crédito: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">operações de crédito para adiantamento de recursos às pessoas jurídicas com base em fluxo de caixa futuro vinculado a direitos creditórios sob a forma de faturas de cartão de crédito
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">outros direitos creditórios descontados: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">operação  de crédito que permite antecipar o valor da venda a prazo dos produtos ou serviços mediante desconto de nota promissória
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outros títulos descontados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: demais títulos descontados</t>
+    </r>
+  </si>
+  <si>
+    <t>Desconto de duplicatas 
+Desconto de cheques
+Antecipação de fatura de cartão de crédito
+Outros direitos creditorios descontados
+Outros títulos descontados</t>
+  </si>
+  <si>
+    <t>O responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Jurídicas cosultadas - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. 
 Deve-se ter apenas os números do CNPJ, sem máscara.</t>
-  </si>
-  <si>
-    <t>Descrição da Remuneração relativa as taxas de juros remuneratórias sobre a modalidade de direitos creditórios descontados infomrada, para pessoa física</t>
-  </si>
-  <si>
-    <t>^(\d{14})$</t>
-  </si>
-  <si>
-    <t>Números de 0 a 9 sem formatação</t>
-  </si>
-  <si>
-    <t>Sigla de identificação do serviço relacionado à Modalidade de direitos creditórios descontados, para pessoa física. Campo aberto. P. ex.  (Trazer a Exemplo)</t>
-  </si>
-  <si>
-    <t>Fatores geradores de cobrança que incidem sobre as Modalidades de direitos creditórios descontados, para pessoa física. Campo Livre Trazer Exemplo</t>
-  </si>
-  <si>
-    <t>^(\W{3}){1}$</t>
-  </si>
-  <si>
-    <t>moeda (ISO-4217)</t>
-  </si>
-  <si>
-    <t>(-?[1-9]?\d{1,2}){1}(\,\d{1,2}){1}</t>
-  </si>
-  <si>
-    <t>^(\d{1})$</t>
-  </si>
-  <si>
-    <t>^(a\.[d,m,a]\.){1}$</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>chargingTriggerInfo</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indica os tipos: mínimo, médio e máximo do valor informado. P.ex.'mínimo' </t>
-  </si>
-  <si>
-    <t>Mínimo
-Médio
-Máximo</t>
-  </si>
-  <si>
-    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para o item priceInfo</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Valor da tarifa cobrada, relativa ao serviço ofertado para a Modalidade de Empréstimo, para pessoa jurídica. P.ex. 45,00</t>
-  </si>
-  <si>
-    <t>Descrição de como é composto o valor da tarifa. p.ex. '0,25% sobre o excedente do limite acima de R$ 500,00'</t>
-  </si>
-  <si>
-    <t>Este campo deve estar obrigatoriamente preenchido se não houver conteúdo para os itens: value, currency e type</t>
-  </si>
-  <si>
-    <t>changingUnit</t>
-  </si>
-  <si>
-    <t>Unidade ou forma de cobrança. P.ex. 'Por mês'</t>
-  </si>
-  <si>
-    <t>este campo sempre deverá estar preenchido</t>
-  </si>
-  <si>
-    <t>^(\d{1,9}\,\d{2}){1}$</t>
-  </si>
-  <si>
-    <t>termsConditions</t>
-  </si>
-  <si>
-    <t>additionalInfo</t>
   </si>
   <si>
     <r>
@@ -835,7 +927,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-antecipação de recebíveis de cartão de crédito: </t>
+antecipação de fatura de cartão de crédito: </t>
     </r>
     <r>
       <rPr>
@@ -855,7 +947,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-desconto de nota promissória: </t>
+outros direitos creditórios descontados: </t>
     </r>
     <r>
       <rPr>
@@ -864,7 +956,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>operação</t>
+      <t>operação  de crédito que permite antecipar o valor da venda a prazo dos produtos ou serviços mediante desconto de nota promissória</t>
     </r>
     <r>
       <rPr>
@@ -874,7 +966,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">
+outros títulos descontados: </t>
     </r>
     <r>
       <rPr>
@@ -883,12 +976,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> de crédito que permite antecipar o valor da venda a prazo dos produtos ou serviços mediante desconto de nota promissória</t>
+      <t>demais títulos descontados</t>
     </r>
   </si>
   <si>
+    <t>O responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Físicas cosultadas - o CNPJ corresponde ao número de inscrição no Cadastro de Pessoa Jurídica. 
+Deve-se ter apenas os números do CNPJ, sem máscara.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Modalidades de direitos creditórios descontados ofertados para pessoas Físicas, conforme Circular 4015-Bacen. Direito creditório descontado é a antecipação de créditos relativos por ex. ao: desconto de duplicatas, desconto de cheques,antecipação de fatura de cartão de crédito
+      <t xml:space="preserve">Relação de garantias exigidas, segundo documento 3040 do Bacen, p.ex.: 
 </t>
     </r>
     <r>
@@ -899,7 +996,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>desconto de duplicatas:</t>
+      <t>cessão de direitos creditórios</t>
     </r>
     <r>
       <rPr>
@@ -908,7 +1005,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a duplicatas mercantis
+      <t xml:space="preserve">: o cedente transfere ao credor/cessionário a titularidade de direitos creditórios, até a liquidação da dívida. O credor/cessionário passa a recebê-los diretamente dos devedores e credita o produto da operação para o cedente na operação que originou a cessão, até a sua liquidação, 
 </t>
     </r>
     <r>
@@ -919,7 +1016,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>desconto de cheques:</t>
+      <t>caução</t>
     </r>
     <r>
       <rPr>
@@ -928,79 +1025,55 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> operações de crédito para adiantamento de recursos com base em fluxo de caixa futuro vinculado a cheques custodiados
+      <t xml:space="preserve">: garantia instituída sobre créditos do garantidor, 
 </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">antecipação de recebíveis de cartão de crédito: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">operações de crédito para adiantamento de recursos às pessoas jurídicas com base em fluxo de caixa futuro vinculado a direitos creditórios sob a forma de faturas de cartão de crédito
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">desconto de nota promissória: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>operação  de crédito que permite antecipar o valor da venda a prazo dos produtos ou serviços mediante desconto de nota promissória</t>
-    </r>
-  </si>
-  <si>
-    <t>Cessão de direitos creditórios
-Caução
-Penhor
-Alienação fiduciária
-Hipoteca
-Operações garantidas pelo governo
-Outras garantias não fidejussórias
-Seguros e assemelhados
-Garantia fidejussória
-Bens arrendados
-Garantias internacionais
-Operações garantidas por outras entidades
-Acordos de compensação
-Não aplicável</t>
-  </si>
-  <si>
-    <t>a.d.
-a.m.
-a.a.</t>
-  </si>
-  <si>
-    <t>Pré
-Pós</t>
+  </si>
+  <si>
+    <t>Nome da Instituição, pertencente à marca, responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Jurídicas cosultadas. Ex. 'Empresa da Organização A'</t>
   </si>
   <si>
     <t>Desconto de duplicatas 
 Desconto de cheques
-Antecipação de recebíveis de cartão de crédito
-Desconto de nota promissória</t>
+Antecipação de fatura de cartão de crédito
+Outros direitos creditórios descontados
+Outros títulos descontados</t>
+  </si>
+  <si>
+    <t>Nome da Instituição, pertencente à marca, responsável pela comercialização das modalidades de direitos creditórios descontados para Pessoas Físicas cosultadas. Ex. 'Empresa da Organização A'</t>
+  </si>
+  <si>
+    <t>Nome da Marca reportada pelo participante do Open Banking. O conceito a que se refere a 'marca' utilizada está em definição pelos participantes.</t>
+  </si>
+  <si>
+    <t>Indica o tipo de valor referente a tarifa do serviço informado: mínimo, 1º quartil de clientes, 2º quartil de clientes, 3º quartil de clientes e 4º quartil de clientes</t>
+  </si>
+  <si>
+    <t>\W*</t>
+  </si>
+  <si>
+    <t>mínimo'
+'1º quartil de clientes'
+'2º quartil de clientes'
+'3º quartil de clientes'
+'4º quartil de clientes'</t>
+  </si>
+  <si>
+    <t>Este campo deve estar obrigatoriamente preenchido</t>
+  </si>
+  <si>
+    <t>Valor da tarifa cobrada, relativa ao serviço ofertado para a Modalidade de Financiamento, para pessoa jurídica. p.ex. 45.00
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
+  </si>
+  <si>
+    <t>Percentual que incide sobre a composição da  taxa de juros remuneratórias
+(representa uma porcentagem Ex: 0.15 (O valor ao lado representa 15%. O valor 1 representa 100%)</t>
+  </si>
+  <si>
+    <t>Números de 0 a 9.</t>
+  </si>
+  <si>
+    <t>Números de 0 a 9</t>
   </si>
 </sst>
 </file>
@@ -1029,12 +1102,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1064,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1123,6 +1202,57 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,13 +1534,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1549,7 @@
     <col min="2" max="2" width="16.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="100.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" style="4" customWidth="1"/>
@@ -1442,7 +1572,7 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="34" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -1465,28 +1595,28 @@
       </c>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/",B2)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/name</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/",B2)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/name</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
+      <c r="C2" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="13">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="12">
-        <v>30</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="13">
@@ -1496,32 +1626,32 @@
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B3)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/name</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/",B3)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/name</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="13">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="12">
-        <v>30</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="13">
@@ -1531,34 +1661,34 @@
         <v>1</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/",B4)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/cnpjNumber</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B4)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/cnpjNumber</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="13">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="12">
-        <v>14</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -1567,531 +1697,535 @@
         <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B5)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/types</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B5)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/types</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="15">
-        <v>50</v>
+        <v>213</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="35">
+        <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="6" t="s">
-        <v>230</v>
+      <c r="H5" s="24" t="s">
+        <v>220</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="13">
-        <v>4</v>
+      <c r="J5" s="37">
+        <v>5</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B6)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/serviceName</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B6)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/serviceName</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="13">
+        <v>50</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="12">
-        <v>50</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="13">
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B7)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/serviceCode</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B7)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/serviceCode</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="13">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="12">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B8)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/chargingTriggerInfo</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B8)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/chargingTriggerInfo</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="12">
+        <v>12</v>
+      </c>
+      <c r="E8" s="13">
         <v>2000</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="13">
         <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/",B9)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/type</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/",B9)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/type</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="12">
-        <v>6</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="I9" s="17">
-        <v>0</v>
-      </c>
-      <c r="J9" s="17">
+        <v>200</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="29">
+        <v>30</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="I9" s="29">
+        <v>5</v>
+      </c>
+      <c r="J9" s="29">
+        <v>5</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/",B10)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/value</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="36">
+        <v>12</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="29">
+        <v>5</v>
+      </c>
+      <c r="J10" s="29">
+        <v>5</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/",B11)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/currency</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="36">
         <v>3</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <f t="shared" ref="A10:A11" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/",B10)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/value</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="F11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="12">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="17">
-        <v>0</v>
-      </c>
-      <c r="J10" s="17">
-        <v>3</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/price/currency</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="12">
-        <v>3</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="17">
-        <v>0</v>
-      </c>
-      <c r="J11" s="17">
-        <v>3</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>214</v>
+      <c r="G11" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="I11" s="29">
+        <v>5</v>
+      </c>
+      <c r="J11" s="29">
+        <v>5</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>226</v>
       </c>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/additionalInfo</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B12)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/additionalInfo</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="12">
+        <v>12</v>
+      </c>
+      <c r="E12" s="13">
         <v>80</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="17">
         <v>0</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B13)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="13">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="12">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="17">
         <v>1</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
-        <f t="shared" ref="A14:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/",B14)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/rate</v>
+        <f t="shared" ref="A14:A19" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B14)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/rate</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13">
+        <v>7</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="12">
-        <v>7</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="13">
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/referencialRate</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referencialRate</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="13">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="12">
-        <v>7</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="G15" s="4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/indexer</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/indexer</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="12">
+        <v>27</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13">
         <v>30</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="13">
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/prePostTax</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/prePostTax</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="12">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="25">
+        <v>10</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/frequency</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/frequency</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="12">
+        <v>33</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="25">
         <v>4</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/interestRates/incomeRateInfo</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="12">
+        <v>12</v>
+      </c>
+      <c r="E19" s="13">
         <v>1000</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="13">
         <v>0</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B20)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="12">
+        <v>218</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="13">
         <v>50</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="14" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -2103,26 +2237,26 @@
     </row>
     <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/",B21)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/personalInvoiceFinancings/termsConditions</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B21)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/termsConditions</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="12">
+        <v>12</v>
+      </c>
+      <c r="E21" s="13">
         <v>2000</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="13">
@@ -2135,7 +2269,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
-      <c r="E22" s="15"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="20"/>
@@ -2152,47 +2286,6 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2204,7 +2297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2263,28 +2356,28 @@
       </c>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/",B2)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/name</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/",B2)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/name</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
+      <c r="C2" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="12">
         <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="13">
@@ -2294,32 +2387,32 @@
         <v>1</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B3)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/name</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/",B3)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/name</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="12">
         <v>30</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="13">
@@ -2329,34 +2422,34 @@
         <v>1</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/",B4)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/cnpjNumber</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/",B4)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/cnpjNumber</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" s="14" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="12">
         <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -2365,524 +2458,532 @@
         <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B5)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/types</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B5)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/types</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>19</v>
+        <v>216</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>12</v>
       </c>
       <c r="E5" s="15">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="6" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="13" t="s">
-        <v>209</v>
+      <c r="J5" s="29">
+        <v>5</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B6)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/serviceName</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B6)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/serviceName</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="12">
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="13">
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B7)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/serviceCode</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B7)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/serviceCode</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="12">
         <v>30</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B8)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/chargingTriggerInfo</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B8)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/chargingTriggerInfo</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="12">
         <v>2000</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/",B9)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/type</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/",B9)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/type</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="12">
-        <v>6</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="I9" s="13">
-        <v>0</v>
-      </c>
-      <c r="J9" s="13">
+        <v>200</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="29">
+        <v>30</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="I9" s="29">
+        <v>5</v>
+      </c>
+      <c r="J9" s="29">
+        <v>5</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/",B10)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/value</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="36">
+        <v>12</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="29">
+        <v>5</v>
+      </c>
+      <c r="J10" s="29">
+        <v>5</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/",B11)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/currency</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="36">
         <v>3</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <f t="shared" ref="A10:A11" si="0">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/",B10)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/value</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="F11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="12">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="13">
-        <v>0</v>
-      </c>
-      <c r="J10" s="13">
-        <v>3</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/price/currency</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="12">
-        <v>3</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0</v>
-      </c>
-      <c r="J11" s="13">
-        <v>3</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>214</v>
+      <c r="G11" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="I11" s="29">
+        <v>5</v>
+      </c>
+      <c r="J11" s="29">
+        <v>5</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/additionalInfo</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B12)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/additionalInfo</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="12">
         <v>80</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="13">
         <v>0</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B13)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="12">
         <v>50</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="13">
         <v>1</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
-        <f t="shared" ref="A14:A19" si="1">CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/",B14)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/rate</v>
+        <f t="shared" ref="A14:A19" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B14)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/rate</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="12">
         <v>7</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="13"/>
+      <c r="I14" s="13">
+        <v>1</v>
+      </c>
       <c r="J14" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/referencialRate</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referencialRate</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="12">
         <v>7</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/indexer</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/indexer</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="E16" s="12">
         <v>30</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="13">
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/prePostTax</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/prePostTax</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="E17" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/frequency</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/frequency</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="E18" s="12">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="H18" s="19" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/interestRates/incomeRateInfo</v>
+        <f t="shared" si="0"/>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="12">
         <v>1000</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="13">
         <v>0</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B20)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
+        <v>190</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="E20" s="12">
         <v>50</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="H20" s="14" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -2894,26 +2995,26 @@
     </row>
     <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/",B21)</f>
-        <v>openBankingBrazil/&lt;organisation&gt;/companies/businessInvoiceFinancings/termsConditions</v>
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B21)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/termsConditions</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="12">
         <v>2000</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="13">
@@ -3006,112 +3107,112 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3135,163 +3236,163 @@
   <sheetData>
     <row r="1" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -3301,142 +3402,142 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
@@ -3447,7 +3548,7 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
@@ -3458,7 +3559,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -3474,157 +3575,157 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
@@ -3634,172 +3735,172 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
@@ -3809,12 +3910,12 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Acrescidos valores de referência absolutos para as taxas praticadas.
Acrescidos valores de referência absolutos para as taxas praticadas.
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Antec Recebíveis.xlsx
+++ b/DicionarioDeDados-Antec Recebíveis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AD477B-29DD-4882-9D3C-020BF6C19B37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C624D2C-CBDD-4F89-8E1E-20CD7EAC4250}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="238">
   <si>
     <t>Xpath</t>
   </si>
@@ -1075,6 +1075,29 @@
   <si>
     <t>Números de 0 a 9</t>
   </si>
+  <si>
+    <t>Identifica o período referente ao percentual de taxa de remuneração efetivamente aplicada no intervalo informado: mínimo, 1º quartil de clientes, 2º quartil de clientes, 3º quartil de clientes e 4º quartil de clientes</t>
+  </si>
+  <si>
+    <t>Valor do percentual que corresponde a taxa de remuneração efetivamente aplicada no intervalo informado
+(representação de uma porcentagem Ex: 0.15 (O valor ao lado representa 15%. O valor 1 representa 100%))</t>
+  </si>
+  <si>
+    <t>Valor de referência utilizado na apuração dos percentuais informados por quartil
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeda relativa ao valor de referência, segundo modelo ISO-4217. p. ex. 'BRL' </t>
+  </si>
+  <si>
+    <t>referenceValue</t>
+  </si>
+  <si>
+    <t>referenceCurrency</t>
+  </si>
 </sst>
 </file>
 
@@ -1102,7 +1125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1112,6 +1135,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,7 +1172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1253,6 +1282,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1534,18 +1581,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71" style="4" customWidth="1"/>
+    <col min="1" max="1" width="90.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="100.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
@@ -2203,89 +2250,229 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B20)</f>
+    <row r="20" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/types</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="38">
+        <v>30</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="41">
+        <v>5</v>
+      </c>
+      <c r="J20" s="41">
+        <v>5</v>
+      </c>
+      <c r="K20" s="38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/",B21)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/rate</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="38">
+        <v>7</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="41">
+        <v>5</v>
+      </c>
+      <c r="J21" s="41">
+        <v>5</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="31" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B22)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referenceValue</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="41">
+        <v>12</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="H22" s="38"/>
+      <c r="I22" s="41">
+        <v>1</v>
+      </c>
+      <c r="J22" s="41">
+        <v>1</v>
+      </c>
+      <c r="K22" s="39" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="31" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B23)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referenceCurrency</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="42">
+        <v>3</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="I23" s="41">
+        <v>1</v>
+      </c>
+      <c r="J23" s="41">
+        <v>1</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B24)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="D24" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="13">
         <v>50</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="14" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="I20" s="13">
-        <v>1</v>
-      </c>
-      <c r="J20" s="13">
+      <c r="I24" s="13">
+        <v>1</v>
+      </c>
+      <c r="J24" s="13">
         <v>14</v>
       </c>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B21)</f>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B25)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/termsConditions</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="13">
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="13">
         <v>2000</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="13">
+      <c r="H25" s="20"/>
+      <c r="I25" s="13">
         <v>0</v>
       </c>
-      <c r="J21" s="13">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="6"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="14"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="6"/>
+      <c r="J25" s="13">
+        <v>1</v>
+      </c>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="14"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2295,18 +2482,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="94.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="100.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
@@ -2316,7 +2503,7 @@
     <col min="8" max="8" width="44" style="4" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" style="14" customWidth="1"/>
+    <col min="11" max="11" width="49.5703125" style="14" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -2659,7 +2846,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/",B11)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/currency</v>
@@ -2959,120 +3146,215 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="210" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B20)</f>
+    <row r="20" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/",B20)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/types</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="38">
+        <v>30</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="38">
+        <v>5</v>
+      </c>
+      <c r="J20" s="38">
+        <v>5</v>
+      </c>
+      <c r="K20" s="38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/",B21)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/rate</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="38">
+        <v>7</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38">
+        <v>5</v>
+      </c>
+      <c r="J21" s="38">
+        <v>5</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B22)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referenceValue</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="38">
+        <v>12</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38">
+        <v>1</v>
+      </c>
+      <c r="J22" s="38">
+        <v>1</v>
+      </c>
+      <c r="K22" s="38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="31" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B23)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referenceCurrency</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="42">
+        <v>3</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="I23" s="38">
+        <v>1</v>
+      </c>
+      <c r="J23" s="38">
+        <v>1</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B24)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="D24" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="12">
         <v>50</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H24" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="I20" s="13">
-        <v>1</v>
-      </c>
-      <c r="J20" s="13">
+      <c r="I24" s="13">
+        <v>1</v>
+      </c>
+      <c r="J24" s="13">
         <v>14</v>
       </c>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B21)</f>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B25)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/termsConditions</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="12">
         <v>2000</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="13">
+      <c r="H25" s="20"/>
+      <c r="I25" s="13">
         <v>0</v>
       </c>
-      <c r="J21" s="13">
-        <v>1</v>
-      </c>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="6"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="14"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+      <c r="J25" s="13">
+        <v>1</v>
+      </c>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="20"/>
@@ -3081,10 +3363,55 @@
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="14"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="20"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Colocado valor de referência absoluto para as tarifas
Colocado valor de referência absoluto para as tarifas
</commit_message>
<xml_diff>
--- a/DicionarioDeDados-Antec Recebíveis.xlsx
+++ b/DicionarioDeDados-Antec Recebíveis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSDS\Documents\GitHub\Open-Banking-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C624D2C-CBDD-4F89-8E1E-20CD7EAC4250}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1F8C484-548C-475B-839E-B39976845E38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AntecRecebíveisPF" sheetId="10" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="242">
   <si>
     <t>Xpath</t>
   </si>
@@ -1046,9 +1046,6 @@
     <t>Nome da Marca reportada pelo participante do Open Banking. O conceito a que se refere a 'marca' utilizada está em definição pelos participantes.</t>
   </si>
   <si>
-    <t>Indica o tipo de valor referente a tarifa do serviço informado: mínimo, 1º quartil de clientes, 2º quartil de clientes, 3º quartil de clientes e 4º quartil de clientes</t>
-  </si>
-  <si>
     <t>\W*</t>
   </si>
   <si>
@@ -1062,10 +1059,6 @@
     <t>Este campo deve estar obrigatoriamente preenchido</t>
   </si>
   <si>
-    <t>Valor da tarifa cobrada, relativa ao serviço ofertado para a Modalidade de Financiamento, para pessoa jurídica. p.ex. 45.00
-(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
-  </si>
-  <si>
     <t>Percentual que incide sobre a composição da  taxa de juros remuneratórias
 (representa uma porcentagem Ex: 0.15 (O valor ao lado representa 15%. O valor 1 representa 100%)</t>
   </si>
@@ -1097,6 +1090,30 @@
   </si>
   <si>
     <t>referenceCurrency</t>
+  </si>
+  <si>
+    <t>Valor de referência utilizado na apuração dos valores informados por quartil
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
+  </si>
+  <si>
+    <t>Indica o período relativo a tarifa do serviço informado: mínimo, 1º quartil de clientes, 2º quartil de clientes, 3º quartil de clientes e 4º quartil de clientes</t>
+  </si>
+  <si>
+    <t>Valor da tarifa, relativa ao serviço ofertado, para pessoa jurídica informado no período. p.ex. '45.00'
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
+  </si>
+  <si>
+    <t>Valor da tarifa, relativa ao serviço ofertado, para pessoa física informado no período. p.ex. '45.00'
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
+  </si>
+  <si>
+    <t>Identifica o período referente ao percentual de taxa de remuneração efetivamente aplicada no intervalo informado: 
+mínimo, 1º quartil de clientes, 2º quartil de clientes, 3º quartil de clientes e 4º quartil de clientes</t>
+  </si>
+  <si>
+    <t>Valor de referência utilizado na apuração dos percentuais informados por quartil
+(representa um valor monetário Ex: 1547368.92 (O valor ao lado, considerando que a moeda seja BRL, significa 
+R$ 1.547.368,92). O único separador presente deverá ser o . (ponto) para casa decimal. Não deve haver separador de milhar)</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1232,9 +1249,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1248,15 +1262,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1264,9 +1269,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1581,13 +1583,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22:B23"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1621,7 @@
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -1650,7 +1652,7 @@
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>222</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1735,7 +1737,7 @@
         <v>192</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -1758,23 +1760,23 @@
       <c r="C5" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="35">
+      <c r="D5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="30">
         <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>220</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="32">
         <v>5</v>
       </c>
       <c r="K5" s="6"/>
@@ -1883,36 +1885,36 @@
       <c r="B9" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="13">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="29">
-        <v>30</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="H9" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="I9" s="13">
+        <v>5</v>
+      </c>
+      <c r="J9" s="13">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="I9" s="29">
-        <v>5</v>
-      </c>
-      <c r="J9" s="29">
-        <v>5</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>226</v>
-      </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/",B10)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/price/value</v>
@@ -1920,30 +1922,30 @@
       <c r="B10" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="36">
-        <v>12</v>
-      </c>
-      <c r="F10" s="27" t="s">
+      <c r="C10" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="13">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="29">
+      <c r="H10" s="5"/>
+      <c r="I10" s="13">
         <v>5</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="13">
         <v>5</v>
       </c>
-      <c r="K10" s="21" t="s">
-        <v>226</v>
+      <c r="K10" s="6" t="s">
+        <v>225</v>
       </c>
       <c r="L10" s="4"/>
     </row>
@@ -1955,524 +1957,596 @@
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="36">
+      <c r="D11" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="31">
         <v>3</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="13">
         <v>5</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="13">
         <v>5</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B12)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/referenceValue</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="36">
+        <v>12</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="36">
+        <v>1</v>
+      </c>
+      <c r="J12" s="36">
+        <v>1</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B13)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/referenceCurrency</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="37">
+        <v>3</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" s="36">
+        <v>1</v>
+      </c>
+      <c r="J13" s="36">
+        <v>1</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B14)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/additionalInfo</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13">
+        <v>80</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B15)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="13">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="17">
+        <v>1</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <f t="shared" ref="A16:A21" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B16)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/rate</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/additionalInfo</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="13">
-        <v>80</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="17">
-        <v>0</v>
-      </c>
-      <c r="J12" s="17" t="s">
+      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13">
+        <v>7</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="13">
+        <v>1</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/fees/changingUnit</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="13">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="17">
-        <v>1</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="str">
-        <f t="shared" ref="A14:A19" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B14)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/rate</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="13">
-        <v>7</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="13">
-        <v>1</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="str">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referencialRate</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="13">
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="13">
         <v>7</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="13">
-        <v>1</v>
-      </c>
-      <c r="J15" s="13" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="13">
+        <v>1</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="str">
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/indexer</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="13">
+      <c r="D18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="13">
         <v>30</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="13">
-        <v>1</v>
-      </c>
-      <c r="J16" s="13" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="13">
+        <v>1</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="str">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/prePostTax</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="25">
+      <c r="D19" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="24">
         <v>10</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H17" s="14" t="s">
+      <c r="G19" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="I17" s="13">
-        <v>1</v>
-      </c>
-      <c r="J17" s="13" t="s">
+      <c r="I19" s="13">
+        <v>1</v>
+      </c>
+      <c r="J19" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="str">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/frequency</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D20" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="24">
         <v>4</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H18" s="19" t="s">
+      <c r="G20" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="I18" s="13">
-        <v>1</v>
-      </c>
-      <c r="J18" s="13" t="s">
+      <c r="I20" s="13">
+        <v>1</v>
+      </c>
+      <c r="J20" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="str">
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="13">
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="13">
         <v>1000</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="13">
+      <c r="H21" s="5"/>
+      <c r="I21" s="13">
         <v>0</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J21" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/",B20)</f>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/",B22)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/types</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B22" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C22" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="33">
+        <v>30</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="I22" s="36">
+        <v>5</v>
+      </c>
+      <c r="J22" s="36">
+        <v>5</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/",B23)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/rate</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="33">
+        <v>7</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="36">
+        <v>5</v>
+      </c>
+      <c r="J23" s="36">
+        <v>5</v>
+      </c>
+      <c r="K23" s="33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B24)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referenceValue</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="38">
-        <v>30</v>
-      </c>
-      <c r="F20" s="38" t="s">
+      <c r="D24" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="36">
+        <v>12</v>
+      </c>
+      <c r="F24" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="H20" s="38" t="s">
+      <c r="G24" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" s="36">
+        <v>1</v>
+      </c>
+      <c r="J24" s="36">
+        <v>1</v>
+      </c>
+      <c r="K24" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="I20" s="41">
-        <v>5</v>
-      </c>
-      <c r="J20" s="41">
-        <v>5</v>
-      </c>
-      <c r="K20" s="38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/",B21)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/application/rate</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="38" t="s">
+    </row>
+    <row r="25" spans="1:11" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B25)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referenceCurrency</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="37">
+        <v>3</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="38">
-        <v>7</v>
-      </c>
-      <c r="F21" s="38" t="s">
+      <c r="I25" s="36">
+        <v>1</v>
+      </c>
+      <c r="J25" s="36">
+        <v>1</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B26)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="13">
+        <v>50</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="41">
-        <v>5</v>
-      </c>
-      <c r="J21" s="41">
-        <v>5</v>
-      </c>
-      <c r="K21" s="38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="31" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B22)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referenceValue</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="41">
-        <v>12</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="41">
-        <v>1</v>
-      </c>
-      <c r="J22" s="41">
-        <v>1</v>
-      </c>
-      <c r="K22" s="39" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="31" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/",B23)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/interestRates/referenceCurrency</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="42">
-        <v>3</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="H23" s="43" t="s">
-        <v>234</v>
-      </c>
-      <c r="I23" s="41">
-        <v>1</v>
-      </c>
-      <c r="J23" s="41">
-        <v>1</v>
-      </c>
-      <c r="K23" s="39" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B24)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/requiredWarranties</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="13">
-        <v>50</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="14" t="s">
+      <c r="G26" s="5"/>
+      <c r="H26" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="I24" s="13">
-        <v>1</v>
-      </c>
-      <c r="J24" s="13">
+      <c r="I26" s="13">
+        <v>1</v>
+      </c>
+      <c r="J26" s="13">
         <v>14</v>
       </c>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B25)</f>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/",B27)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/personalInvoiceFinancings/termsConditions</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="13">
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="13">
         <v>2000</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="13">
+      <c r="H27" s="20"/>
+      <c r="I27" s="13">
         <v>0</v>
       </c>
-      <c r="J25" s="13">
-        <v>1</v>
-      </c>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="6"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="14"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="J27" s="13">
+        <v>1</v>
+      </c>
       <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="14"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2482,20 +2556,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="112.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="12" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" style="4" customWidth="1"/>
@@ -2551,7 +2625,7 @@
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>222</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2636,7 +2710,7 @@
         <v>192</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -2659,7 +2733,7 @@
       <c r="C5" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="21" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="15">
@@ -2675,7 +2749,7 @@
       <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="25">
         <v>5</v>
       </c>
       <c r="K5" s="6"/>
@@ -2784,35 +2858,35 @@
       <c r="B9" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="13">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="29">
-        <v>30</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="H9" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="I9" s="13">
+        <v>5</v>
+      </c>
+      <c r="J9" s="13">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="I9" s="29">
-        <v>5</v>
-      </c>
-      <c r="J9" s="29">
-        <v>5</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/",B10)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/price/value</v>
@@ -2820,30 +2894,30 @@
       <c r="B10" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="36">
-        <v>12</v>
-      </c>
-      <c r="F10" s="27" t="s">
+      <c r="C10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="13">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="29">
+      <c r="H10" s="5"/>
+      <c r="I10" s="13">
         <v>5</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="13">
         <v>5</v>
       </c>
-      <c r="K10" s="21" t="s">
-        <v>226</v>
+      <c r="K10" s="6" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2854,526 +2928,575 @@
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="36">
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13">
         <v>3</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="13">
         <v>5</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="13">
         <v>5</v>
       </c>
-      <c r="K11" s="21" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="K11" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B12)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/additionalInfo</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="12">
-        <v>80</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="13">
-        <v>0</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>203</v>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/referenceValue</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="36">
+        <v>12</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="36">
+        <v>1</v>
+      </c>
+      <c r="J12" s="36">
+        <v>1</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B13)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="12">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/referenceCurrency</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="37">
+        <v>3</v>
+      </c>
+      <c r="F13" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" s="36">
+        <v>1</v>
+      </c>
+      <c r="J13" s="36">
+        <v>1</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B14)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/additionalInfo</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="12">
+        <v>80</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="str">
-        <f t="shared" ref="A14:A19" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B14)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/rate</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="12">
-        <v>7</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/",B15)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/fees/changingUnit</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="12">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="13">
+        <v>1</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <f t="shared" ref="A16:A21" si="0">CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B16)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/rate</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="12">
+        <v>7</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="13">
+        <v>1</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referencialRate</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="12">
         <v>7</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="13">
-        <v>1</v>
-      </c>
-      <c r="J15" s="13" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="13">
+        <v>1</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="str">
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/indexer</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12">
         <v>30</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="13">
-        <v>1</v>
-      </c>
-      <c r="J16" s="13" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="13">
+        <v>1</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="str">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/prePostTax</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="D19" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="12">
         <v>10</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H17" s="14" t="s">
+      <c r="G19" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="I17" s="13">
-        <v>1</v>
-      </c>
-      <c r="J17" s="13" t="s">
+      <c r="I19" s="13">
+        <v>1</v>
+      </c>
+      <c r="J19" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="str">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/frequency</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="D20" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="12">
         <v>4</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H18" s="19" t="s">
+      <c r="G20" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="I18" s="13">
-        <v>1</v>
-      </c>
-      <c r="J18" s="13" t="s">
+      <c r="I20" s="13">
+        <v>1</v>
+      </c>
+      <c r="J20" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="str">
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/incomeRateInfo</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="12">
         <v>1000</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="13">
+      <c r="H21" s="5"/>
+      <c r="I21" s="13">
         <v>0</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J21" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/",B20)</f>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/",B22)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/types</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B22" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="38">
+      <c r="C22" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="33">
         <v>30</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F22" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G22" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="H22" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="I22" s="33">
+        <v>5</v>
+      </c>
+      <c r="J22" s="33">
+        <v>5</v>
+      </c>
+      <c r="K22" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="I20" s="38">
+    </row>
+    <row r="23" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/",B23)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/rate</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="33">
+        <v>7</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33">
         <v>5</v>
       </c>
-      <c r="J20" s="38">
+      <c r="J23" s="33">
         <v>5</v>
       </c>
-      <c r="K20" s="38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/",B21)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/application/rate</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="38" t="s">
+      <c r="K23" s="33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B24)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referenceValue</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="33">
+        <v>12</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33">
+        <v>1</v>
+      </c>
+      <c r="J24" s="33">
+        <v>1</v>
+      </c>
+      <c r="K24" s="33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="27" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B25)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referenceCurrency</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="37">
+        <v>3</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="38">
-        <v>7</v>
-      </c>
-      <c r="F21" s="38" t="s">
+      <c r="I25" s="33">
+        <v>1</v>
+      </c>
+      <c r="J25" s="33">
+        <v>1</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B26)</f>
+        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="12">
+        <v>50</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38">
-        <v>5</v>
-      </c>
-      <c r="J21" s="38">
-        <v>5</v>
-      </c>
-      <c r="K21" s="38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B22)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referenceValue</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="38">
-        <v>12</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38">
-        <v>1</v>
-      </c>
-      <c r="J22" s="38">
-        <v>1</v>
-      </c>
-      <c r="K22" s="38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="31" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/",B23)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/interestRates/referenceCurrency</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>237</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="42">
-        <v>3</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="H23" s="43" t="s">
-        <v>234</v>
-      </c>
-      <c r="I23" s="38">
-        <v>1</v>
-      </c>
-      <c r="J23" s="38">
-        <v>1</v>
-      </c>
-      <c r="K23" s="39" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="210" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B24)</f>
-        <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/requiredWarranties</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="12">
-        <v>50</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H26" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="I24" s="13">
-        <v>1</v>
-      </c>
-      <c r="J24" s="13">
+      <c r="I26" s="13">
+        <v>1</v>
+      </c>
+      <c r="J26" s="13">
         <v>14</v>
       </c>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="str">
-        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B25)</f>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="str">
+        <f>CONCATENATE("openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/",B27)</f>
         <v>openBankingBrazil/&lt;brand&gt;/companies/businessInvoiceFinancings/termsConditions</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="12">
         <v>2000</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="13">
+      <c r="H27" s="20"/>
+      <c r="I27" s="13">
         <v>0</v>
       </c>
-      <c r="J25" s="13">
-        <v>1</v>
-      </c>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="6"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="14"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="J27" s="13">
+        <v>1</v>
+      </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="6"/>
       <c r="E28" s="15"/>
       <c r="F28" s="5"/>
@@ -3384,10 +3507,8 @@
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="14"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="20"/>
@@ -3395,11 +3516,10 @@
       <c r="J29" s="13"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="20"/>
@@ -3408,10 +3528,34 @@
       <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="20"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>